<commit_message>
Ft account expiration (#537)
- 新增: 账号过期时间
- 新增: 新增账户冻结周期任务
- 新增: 密码过期提醒
- bugfix:  DDE注入漏洞解决，设置导入导出模板单元格为文本模式

Co-authored-by: Canway-shiisa <90179140+Canway-shiisa@users.noreply.github.com>
Co-authored-by: v_yutyi <v_yutyi@tencent.com>
Co-authored-by: Canway-jessonwang <101160580+Canway-jessonwang@users.noreply.github.com>
Co-authored-by: nero <nero@canway.net>
</commit_message>
<xml_diff>
--- a/src/saas/media/excel/export_org_tmpl.xlsx
+++ b/src/saas/media/excel/export_org_tmpl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amazingblues/SourceCode/BlueKing/bk-user/src/saas/media/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CanwayProject\bkuser_dev\bk-user\src\saas\media\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B62E909-873A-6D49-8419-FB610E150041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4F696D-76DC-4318-9165-414CD0C4490C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>用户名</t>
   </si>
@@ -124,12 +124,16 @@
     <t>账户状态</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>账号过期时间</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -583,13 +587,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="10" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="10" customWidth="1"/>
@@ -597,14 +601,14 @@
     <col min="4" max="4" width="19.33203125" style="10" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" style="10" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="22" style="4" customWidth="1"/>
-    <col min="9" max="9" width="39.1640625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="17" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="28.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22" style="4" customWidth="1"/>
+    <col min="10" max="10" width="39.1640625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="17" style="4" customWidth="1"/>
+    <col min="12" max="12" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="251" customHeight="1">
+    <row r="1" spans="1:13" ht="251" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -618,9 +622,10 @@
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="33.75" customHeight="1">
+      <c r="L1" s="11"/>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -642,320 +647,323 @@
       <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9">
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51041666666666696" footer="0.51041666666666696"/>

</xml_diff>